<commit_message>
Constrain level-1 fields in lightsheet
</commit_message>
<xml_diff>
--- a/docs/lightsheet/lightsheet-metadata.xlsx
+++ b/docs/lightsheet/lightsheet-metadata.xlsx
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>donor_id</t>
   </si>
@@ -387,130 +387,16 @@
     <t>imaging</t>
   </si>
   <si>
-    <t>mass_spectrometry</t>
-  </si>
-  <si>
-    <t>mass_spectrometry_imaging</t>
-  </si>
-  <si>
-    <t>sequence</t>
-  </si>
-  <si>
     <t>assay_type</t>
   </si>
   <si>
-    <t>scRNA-Seq (10xGenomics)</t>
-  </si>
-  <si>
-    <t>AF</t>
-  </si>
-  <si>
-    <t>bulk RNA</t>
-  </si>
-  <si>
-    <t>bulkATACseq</t>
-  </si>
-  <si>
-    <t>Cell DIVE</t>
-  </si>
-  <si>
-    <t>CODEX</t>
-  </si>
-  <si>
-    <t>Imaging Mass Cytometry</t>
-  </si>
-  <si>
-    <t>LC-MS (metabolomics)</t>
-  </si>
-  <si>
-    <t>LC-MS/MS (label-free proteomics)</t>
-  </si>
-  <si>
-    <t>MxIF</t>
-  </si>
-  <si>
-    <t>MALDI-IMS</t>
-  </si>
-  <si>
-    <t>MS (shotgun lipidomics)</t>
-  </si>
-  <si>
-    <t>NanoDESI</t>
-  </si>
-  <si>
-    <t>NanoPOTS</t>
-  </si>
-  <si>
-    <t>PAS microscopy</t>
-  </si>
-  <si>
-    <t>scATACseq</t>
-  </si>
-  <si>
-    <t>sciATACseq</t>
-  </si>
-  <si>
-    <t>sciRNAseq</t>
-  </si>
-  <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>SNARE-seq2</t>
-  </si>
-  <si>
-    <t>snATACseq</t>
-  </si>
-  <si>
-    <t>snRNA</t>
-  </si>
-  <si>
-    <t>SPLiT-Seq</t>
-  </si>
-  <si>
-    <t>TMT (proteomics)</t>
-  </si>
-  <si>
-    <t>WGS</t>
-  </si>
-  <si>
-    <t>SNARE2-RNAseq</t>
-  </si>
-  <si>
-    <t>snRNAseq</t>
-  </si>
-  <si>
-    <t>scRNAseq-10xGenomics</t>
-  </si>
-  <si>
-    <t>scRNAseq</t>
-  </si>
-  <si>
-    <t>Slide-seq</t>
+    <t>Light Sheet</t>
   </si>
   <si>
     <t>analyte_class</t>
   </si>
   <si>
-    <t>DNA</t>
-  </si>
-  <si>
-    <t>RNA</t>
-  </si>
-  <si>
     <t>protein</t>
-  </si>
-  <si>
-    <t>lipids</t>
-  </si>
-  <si>
-    <t>metabolites</t>
-  </si>
-  <si>
-    <t>polysaccharides</t>
-  </si>
-  <si>
-    <t>metabolites_and_lipids</t>
   </si>
   <si>
     <t>is_targeted</t>
@@ -945,64 +831,64 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging / mass_spectrometry / mass_spectrometry_imaging / sequence." sqref="I2:I1048576">
-      <formula1>'assay_category list'!$A$1:$A$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="J2:J1048576">
-      <formula1>'assay_type list'!$A$1:$A$30</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from analyte_class list." sqref="K2:K1048576">
-      <formula1>'analyte_class list'!$A$1:$A$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="I2:I1048576">
+      <formula1>'assay_category list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Light Sheet." sqref="J2:J1048576">
+      <formula1>'assay_type list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: protein." sqref="K2:K1048576">
+      <formula1>'analyte_class list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
       <formula1>"TRUE,FALSE"</formula1>
@@ -1044,7 +930,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1055,21 +941,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1077,7 +948,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1085,152 +956,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1240,7 +966,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1248,37 +974,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1296,12 +992,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1319,12 +1015,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1342,12 +1038,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move changes to v2; regen
</commit_message>
<xml_diff>
--- a/docs/lightsheet/lightsheet-metadata.xlsx
+++ b/docs/lightsheet/lightsheet-metadata.xlsx
@@ -14,7 +14,8 @@
     <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
     <sheet name="resolution_x_unit list" sheetId="6" r:id="rId6"/>
     <sheet name="resolution_y_unit list" sheetId="7" r:id="rId7"/>
-    <sheet name="resolution_z_unit list" sheetId="8" r:id="rId8"/>
+    <sheet name="range_z_unit list" sheetId="8" r:id="rId8"/>
+    <sheet name="increment_z_unit list" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -295,7 +296,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The distance at which two objects along the detection z-axis can be distinguished (resolved as 2 objects).</t>
+          <t>The total range of the z axis.</t>
         </r>
       </text>
     </comment>
@@ -308,7 +309,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of z resolution.</t>
+          <t>The unit of range_z_value.</t>
         </r>
       </text>
     </comment>
@@ -321,11 +322,50 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>The number of optical sections in z axis range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The distance between sequential optical sections.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The units of increment z value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Number of antibodies</t>
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -364,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -382,12 +422,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>description</t>
@@ -462,10 +502,19 @@
     <t>resolution_y_unit</t>
   </si>
   <si>
-    <t>resolution_z_value</t>
-  </si>
-  <si>
-    <t>resolution_z_unit</t>
+    <t>range_z_value</t>
+  </si>
+  <si>
+    <t>range_z_unit</t>
+  </si>
+  <si>
+    <t>step_z_value</t>
+  </si>
+  <si>
+    <t>increment_z_value</t>
+  </si>
+  <si>
+    <t>increment_z_unit</t>
   </si>
   <si>
     <t>number_of_antibodies</t>
@@ -829,7 +878,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -838,7 +887,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,10 +969,19 @@
       <c r="AA1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+  <dataValidations count="16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="K2:K1048576">
@@ -957,13 +1015,24 @@
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="V2:V1048576">
-      <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="W2:W1048576">
+      <formula1>'range_z_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="W2:W1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="X2:X1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="Y2:Y1048576">
+      <formula1>'increment_z_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="Z2:Z1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="X2:X1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AA2:AA1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
@@ -1112,4 +1181,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Lightsheet z axis specs, # of sections & increments (#863)
* Update Lightsheet z axis specs, # of sections & increments

Seth Curlin revised the Z resolution fields to more accurate terms for the z dimension in lightsheet image capture:
range_z_value & unit - total z distance captured
step_z_value - number of sections captured
increment_z_value & unit - distance between sections

* move changes to v2; regen

* changelog

Co-authored-by: mccalluc <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/lightsheet/lightsheet-metadata.xlsx
+++ b/docs/lightsheet/lightsheet-metadata.xlsx
@@ -14,7 +14,8 @@
     <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
     <sheet name="resolution_x_unit list" sheetId="6" r:id="rId6"/>
     <sheet name="resolution_y_unit list" sheetId="7" r:id="rId7"/>
-    <sheet name="resolution_z_unit list" sheetId="8" r:id="rId8"/>
+    <sheet name="range_z_unit list" sheetId="8" r:id="rId8"/>
+    <sheet name="increment_z_unit list" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -295,7 +296,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The distance at which two objects along the detection z-axis can be distinguished (resolved as 2 objects).</t>
+          <t>The total range of the z axis.</t>
         </r>
       </text>
     </comment>
@@ -308,7 +309,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of z resolution.</t>
+          <t>The unit of range_z_value.</t>
         </r>
       </text>
     </comment>
@@ -321,11 +322,50 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>The number of optical sections in z axis range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The distance between sequential optical sections.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The units of increment z value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Number of antibodies</t>
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -364,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -382,12 +422,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>description</t>
@@ -462,10 +502,19 @@
     <t>resolution_y_unit</t>
   </si>
   <si>
-    <t>resolution_z_value</t>
-  </si>
-  <si>
-    <t>resolution_z_unit</t>
+    <t>range_z_value</t>
+  </si>
+  <si>
+    <t>range_z_unit</t>
+  </si>
+  <si>
+    <t>step_z_value</t>
+  </si>
+  <si>
+    <t>increment_z_value</t>
+  </si>
+  <si>
+    <t>increment_z_unit</t>
   </si>
   <si>
     <t>number_of_antibodies</t>
@@ -829,7 +878,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -838,7 +887,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,10 +969,19 @@
       <c r="AA1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+  <dataValidations count="16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="K2:K1048576">
@@ -957,13 +1015,24 @@
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="V2:V1048576">
-      <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="W2:W1048576">
+      <formula1>'range_z_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="W2:W1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="X2:X1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="Y2:Y1048576">
+      <formula1>'increment_z_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="Z2:Z1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="X2:X1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AA2:AA1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
@@ -1112,4 +1181,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>